<commit_message>
All changes as of 7-27
</commit_message>
<xml_diff>
--- a/Codebook.xlsx
+++ b/Codebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brockfamily/Documents/SMU/Liminal_Cities_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5D107B0-43FA-49B9-BDEB-75262550E5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB95797B-0D54-4651-AD92-7E18AB0C07CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{F3E93D28-CD45-7145-B5DD-F5A1D6448FDA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="338">
   <si>
     <t>column name</t>
   </si>
@@ -954,6 +954,72 @@
   </si>
   <si>
     <t>B06009_006E</t>
+  </si>
+  <si>
+    <t>Pop_Worked_Home</t>
+  </si>
+  <si>
+    <t>B08119_055E</t>
+  </si>
+  <si>
+    <t>MEANS OF TRANSPORTATION TO WORK BY WORKERS' EARNINGS IN THE PAST 12 MONTHS (IN 2021 INFLATION-ADJUSTED DOLLARS)</t>
+  </si>
+  <si>
+    <t>Pop_Worked_Home_1-10k</t>
+  </si>
+  <si>
+    <t>B08119_056E</t>
+  </si>
+  <si>
+    <t>Pop_Worked_Home_10k-15k</t>
+  </si>
+  <si>
+    <t>B08119_057E</t>
+  </si>
+  <si>
+    <t>Pop_Worked_Home_15k-25k</t>
+  </si>
+  <si>
+    <t>B08119_058E</t>
+  </si>
+  <si>
+    <t>Pop_Worked_Home_25k-35k</t>
+  </si>
+  <si>
+    <t>B08119_059E</t>
+  </si>
+  <si>
+    <t>Pop_Worked_Home_35k-50k</t>
+  </si>
+  <si>
+    <t>B08119_060E</t>
+  </si>
+  <si>
+    <t>Pop_Worked_Home_50k-65k</t>
+  </si>
+  <si>
+    <t>B08119_061E</t>
+  </si>
+  <si>
+    <t>Pop_Worked_Home_65k-75k</t>
+  </si>
+  <si>
+    <t>B08119_062E</t>
+  </si>
+  <si>
+    <t>Pop_Worked_Home_75k-more</t>
+  </si>
+  <si>
+    <t>B08119_063E</t>
+  </si>
+  <si>
+    <t>Median_Income_Worked_home</t>
+  </si>
+  <si>
+    <t>B08121_007E</t>
+  </si>
+  <si>
+    <t>MEDIAN EARNINGS IN THE PAST 12 MONTHS (IN 2021 INFLATION-ADJUSTED DOLLARS) BY MEANS OF TRANSPORTATION TO WORK</t>
   </si>
   <si>
     <t>Less_High_pct</t>
@@ -1420,11 +1486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF32701-AF16-CF40-B6F7-F0E226B7F5D3}">
-  <dimension ref="A1:J125"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A113" sqref="A113:XFD113"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H124" sqref="H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
@@ -3912,28 +3978,28 @@
         <v>274</v>
       </c>
     </row>
-    <row r="99" spans="1:10" s="18" customFormat="1">
-      <c r="A99" s="17" t="s">
+    <row r="99" spans="1:10">
+      <c r="A99" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="B99" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C99" s="17" t="s">
+      <c r="B99" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="D99" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17">
-        <v>927</v>
-      </c>
-      <c r="G99" s="17"/>
-      <c r="H99" s="17" t="s">
+      <c r="D99" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3">
+        <v>927</v>
+      </c>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J99" s="17" t="s">
+      <c r="J99" s="3" t="s">
         <v>277</v>
       </c>
     </row>
@@ -4210,115 +4276,345 @@
       </c>
       <c r="J112" s="3"/>
     </row>
-    <row r="113" spans="1:10" s="10" customFormat="1">
-      <c r="A113" s="9" t="s">
+    <row r="113" spans="1:10" s="18" customFormat="1">
+      <c r="A113" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="B113" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C113" s="10" t="s">
+      <c r="B113" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C113" s="18" t="s">
         <v>305</v>
       </c>
-      <c r="D113" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E113" s="9"/>
-      <c r="F113" s="9"/>
-      <c r="G113" s="9"/>
-      <c r="H113" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J113" s="9"/>
-    </row>
-    <row r="114" spans="1:10">
-      <c r="A114" t="s">
+      <c r="D113" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E113" s="17"/>
+      <c r="F113" s="17"/>
+      <c r="G113" s="17"/>
+      <c r="H113" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J113" s="17"/>
+    </row>
+    <row r="114" spans="1:10" s="18" customFormat="1">
+      <c r="A114" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C114" s="18" t="s">
         <v>307</v>
       </c>
-      <c r="F114">
-        <v>927</v>
-      </c>
-      <c r="J114" t="s">
+      <c r="D114" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E114" s="17"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J114" s="17" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
-      <c r="A115" t="s">
+    <row r="115" spans="1:10" s="18" customFormat="1">
+      <c r="A115" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="B115" t="s">
-        <v>307</v>
-      </c>
-      <c r="F115">
-        <v>927</v>
-      </c>
-      <c r="J115" t="s">
+      <c r="B115" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C115" s="18" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="116" spans="1:10">
-      <c r="A116" t="s">
+      <c r="D115" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E115" s="17"/>
+      <c r="F115" s="17"/>
+      <c r="G115" s="17"/>
+      <c r="H115" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J115" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" s="18" customFormat="1">
+      <c r="A116" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="B116" t="s">
-        <v>307</v>
-      </c>
-      <c r="F116">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10">
-      <c r="A117" t="s">
+      <c r="B116" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C116" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="B117" t="s">
-        <v>307</v>
-      </c>
-      <c r="F117">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10">
-      <c r="A118" t="s">
+      <c r="D116" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E116" s="17"/>
+      <c r="F116" s="17"/>
+      <c r="G116" s="17"/>
+      <c r="H116" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J116" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" s="18" customFormat="1">
+      <c r="A117" s="17" t="s">
         <v>313</v>
       </c>
-      <c r="B118" t="s">
-        <v>307</v>
-      </c>
-      <c r="F118">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10">
-      <c r="A119" t="s">
+      <c r="B117" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C117" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="B119" t="s">
-        <v>307</v>
-      </c>
-      <c r="F119">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10">
-      <c r="A120" t="s">
+      <c r="D117" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" s="17"/>
+      <c r="F117" s="17"/>
+      <c r="G117" s="17"/>
+      <c r="H117" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J117" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" s="18" customFormat="1">
+      <c r="A118" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="B120" t="s">
-        <v>307</v>
-      </c>
-      <c r="F120">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10"/>
-    <row r="122" spans="1:10"/>
-    <row r="123" spans="1:10"/>
-    <row r="124" spans="1:10"/>
-    <row r="125" spans="1:10"/>
+      <c r="B118" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C118" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="D118" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E118" s="17"/>
+      <c r="F118" s="17"/>
+      <c r="G118" s="17"/>
+      <c r="H118" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J118" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" s="18" customFormat="1">
+      <c r="A119" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="B119" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C119" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="D119" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E119" s="17"/>
+      <c r="F119" s="17"/>
+      <c r="G119" s="17"/>
+      <c r="H119" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J119" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" s="18" customFormat="1">
+      <c r="A120" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="B120" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C120" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="D120" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E120" s="17"/>
+      <c r="F120" s="17"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J120" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" s="18" customFormat="1">
+      <c r="A121" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="B121" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C121" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="D121" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E121" s="17"/>
+      <c r="F121" s="17"/>
+      <c r="G121" s="17"/>
+      <c r="H121" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J121" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" s="18" customFormat="1">
+      <c r="A122" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="B122" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C122" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="D122" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E122" s="17"/>
+      <c r="F122" s="17"/>
+      <c r="G122" s="17"/>
+      <c r="H122" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J122" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" s="10" customFormat="1">
+      <c r="A123" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C123" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="D123" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="9"/>
+      <c r="H123" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="J123" s="9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124" t="s">
+        <v>328</v>
+      </c>
+      <c r="B124" t="s">
+        <v>329</v>
+      </c>
+      <c r="F124">
+        <v>927</v>
+      </c>
+      <c r="J124" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" t="s">
+        <v>331</v>
+      </c>
+      <c r="B125" t="s">
+        <v>329</v>
+      </c>
+      <c r="F125">
+        <v>927</v>
+      </c>
+      <c r="J125" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="A126" t="s">
+        <v>333</v>
+      </c>
+      <c r="B126" t="s">
+        <v>329</v>
+      </c>
+      <c r="F126">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="A127" t="s">
+        <v>334</v>
+      </c>
+      <c r="B127" t="s">
+        <v>329</v>
+      </c>
+      <c r="F127">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="A128" t="s">
+        <v>335</v>
+      </c>
+      <c r="B128" t="s">
+        <v>329</v>
+      </c>
+      <c r="F128">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" t="s">
+        <v>336</v>
+      </c>
+      <c r="B129" t="s">
+        <v>329</v>
+      </c>
+      <c r="F129">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" t="s">
+        <v>337</v>
+      </c>
+      <c r="B130" t="s">
+        <v>329</v>
+      </c>
+      <c r="F130">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6"/>
+    <row r="132" spans="1:6"/>
+    <row r="133" spans="1:6"/>
+    <row r="134" spans="1:6"/>
+    <row r="135" spans="1:6"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{1F865059-C1A9-4314-9F76-0A615D19AF0B}"/>

</xml_diff>

<commit_message>
Combine 2010, 15, 19, 20, 21 CSVs to 1 xlsx
</commit_message>
<xml_diff>
--- a/Codebook.xlsx
+++ b/Codebook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26920"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brockfamily/Documents/SMU/Liminal_Cities_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB95797B-0D54-4651-AD92-7E18AB0C07CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C9BA6F4-6E8E-4290-BFC4-EB8772600DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{F3E93D28-CD45-7145-B5DD-F5A1D6448FDA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="338">
   <si>
     <t>column name</t>
   </si>
@@ -152,7 +152,7 @@
     <t>Percent of working population that commutes to a nearby metro</t>
   </si>
   <si>
-    <t xml:space="preserve">liminal </t>
+    <t>liminal</t>
   </si>
   <si>
     <t>True if within 100 mile proximity to metro with pop &gt; 1,000,000, &lt;100,000 in population, and &gt; 5% of workforce commuting to metro</t>
@@ -248,25 +248,25 @@
     <t>(Carbon Monoxide) These columns give the number of days each pollutant measured was the main pollutant</t>
   </si>
   <si>
-    <t xml:space="preserve"> Days NO2</t>
+    <t>Days NO2</t>
   </si>
   <si>
     <t>(Nitrogen dioxide)These columns give the number of days each pollutant measured was the main pollutant</t>
   </si>
   <si>
-    <t xml:space="preserve"> Days Ozone</t>
+    <t>Days Ozone</t>
   </si>
   <si>
     <t>(Ozone)These columns give the number of days each pollutant measured was the main pollutant</t>
   </si>
   <si>
-    <t xml:space="preserve"> Days PM2.5</t>
+    <t>Days PM2.5</t>
   </si>
   <si>
     <t>(Fine Particles)These columns give the number of days each pollutant measured was the main pollutant</t>
   </si>
   <si>
-    <t xml:space="preserve"> Days PM10</t>
+    <t>Days PM10</t>
   </si>
   <si>
     <t>(inhalable particles )These columns give the number of days each pollutant measured was the main pollutant</t>
@@ -335,6 +335,9 @@
     <t>RBIRTH</t>
   </si>
   <si>
+    <t>2015, 2019, 2021</t>
+  </si>
+  <si>
     <t>weighted avg</t>
   </si>
   <si>
@@ -1022,7 +1025,7 @@
     <t>MEDIAN EARNINGS IN THE PAST 12 MONTHS (IN 2021 INFLATION-ADJUSTED DOLLARS) BY MEANS OF TRANSPORTATION TO WORK</t>
   </si>
   <si>
-    <t>Less_High_pct</t>
+    <t>Pct_Less_HS</t>
   </si>
   <si>
     <t>derived from ACS</t>
@@ -1031,25 +1034,22 @@
     <t>Count variable: B20004_002E</t>
   </si>
   <si>
-    <t>High_Equiv_pct</t>
+    <t>Pct_HS_Grad</t>
   </si>
   <si>
     <t>Count variable: B20004_003E</t>
   </si>
   <si>
-    <t>College_Assoc_Equiv_pct</t>
-  </si>
-  <si>
-    <t>Bachelors_pct</t>
-  </si>
-  <si>
-    <t>Grad_Prof_pct</t>
-  </si>
-  <si>
-    <t>Bach_and_Above_pct</t>
-  </si>
-  <si>
-    <t>Computer_Total</t>
+    <t>Pct_Some_College</t>
+  </si>
+  <si>
+    <t>Pct_Bachelors</t>
+  </si>
+  <si>
+    <t>Pct_Grad</t>
+  </si>
+  <si>
+    <t>Pct_BS_Above</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1169,8 +1169,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1489,8 +1487,8 @@
   <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H124" sqref="H124"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F130" sqref="A130:F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
@@ -2453,7 +2451,7 @@
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4">
@@ -2461,25 +2459,25 @@
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>80</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="53.25">
       <c r="A39" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4">
@@ -2487,25 +2485,25 @@
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>80</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="70.5">
       <c r="A40" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4">
@@ -2513,25 +2511,25 @@
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>80</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="70.5">
       <c r="A41" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4">
@@ -2539,25 +2537,25 @@
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>80</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="70.5">
       <c r="A42" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
@@ -2565,25 +2563,25 @@
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I42" s="6" t="s">
         <v>80</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="10" customFormat="1" ht="53.25">
       <c r="A43" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="11">
@@ -2591,53 +2589,53 @@
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I43" s="13" t="s">
         <v>80</v>
       </c>
       <c r="J43" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3">
         <v>938</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I44" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3">
@@ -2645,25 +2643,25 @@
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I45" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3">
@@ -2671,25 +2669,25 @@
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3">
@@ -2700,22 +2698,22 @@
         <v>79</v>
       </c>
       <c r="I47" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="10" customFormat="1">
       <c r="A48" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9">
@@ -2726,18 +2724,18 @@
         <v>79</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J48" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="4" t="s">
@@ -2750,18 +2748,18 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="4" t="s">
@@ -2774,18 +2772,18 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="4" t="s">
@@ -2798,18 +2796,18 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="10" customFormat="1">
       <c r="A52" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="11" t="s">
@@ -2822,21 +2820,21 @@
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
       <c r="I52" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>42</v>
@@ -2850,18 +2848,18 @@
         <v>79</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>42</v>
@@ -2875,18 +2873,18 @@
         <v>79</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>42</v>
@@ -2900,18 +2898,18 @@
         <v>79</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>42</v>
@@ -2922,21 +2920,21 @@
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>42</v>
@@ -2947,21 +2945,21 @@
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>42</v>
@@ -2972,21 +2970,21 @@
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>42</v>
@@ -3000,18 +2998,18 @@
         <v>79</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>42</v>
@@ -3025,18 +3023,18 @@
         <v>79</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>42</v>
@@ -3050,18 +3048,18 @@
         <v>79</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>42</v>
@@ -3075,18 +3073,18 @@
         <v>79</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>42</v>
@@ -3100,18 +3098,18 @@
         <v>79</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>42</v>
@@ -3122,21 +3120,21 @@
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>42</v>
@@ -3147,21 +3145,21 @@
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>42</v>
@@ -3172,21 +3170,21 @@
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>42</v>
@@ -3197,21 +3195,21 @@
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>42</v>
@@ -3222,21 +3220,21 @@
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>42</v>
@@ -3247,21 +3245,21 @@
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>42</v>
@@ -3272,21 +3270,21 @@
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>42</v>
@@ -3297,21 +3295,21 @@
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>42</v>
@@ -3322,21 +3320,21 @@
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>42</v>
@@ -3347,21 +3345,21 @@
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>42</v>
@@ -3372,21 +3370,21 @@
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>42</v>
@@ -3397,21 +3395,21 @@
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>42</v>
@@ -3422,21 +3420,21 @@
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>42</v>
@@ -3447,21 +3445,21 @@
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>42</v>
@@ -3472,21 +3470,21 @@
       </c>
       <c r="G78" s="3"/>
       <c r="H78" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>42</v>
@@ -3497,21 +3495,21 @@
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>42</v>
@@ -3522,21 +3520,21 @@
       </c>
       <c r="G80" s="3"/>
       <c r="H80" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>42</v>
@@ -3547,21 +3545,21 @@
       </c>
       <c r="G81" s="3"/>
       <c r="H81" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>42</v>
@@ -3572,21 +3570,21 @@
       </c>
       <c r="G82" s="3"/>
       <c r="H82" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>42</v>
@@ -3597,21 +3595,21 @@
       </c>
       <c r="G83" s="3"/>
       <c r="H83" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>42</v>
@@ -3622,21 +3620,21 @@
       </c>
       <c r="G84" s="3"/>
       <c r="H84" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>42</v>
@@ -3647,21 +3645,21 @@
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>42</v>
@@ -3672,21 +3670,21 @@
       </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>42</v>
@@ -3697,21 +3695,21 @@
       </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>42</v>
@@ -3722,24 +3720,24 @@
       </c>
       <c r="G88" s="3"/>
       <c r="H88" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3">
@@ -3750,21 +3748,21 @@
         <v>79</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3">
@@ -3775,21 +3773,21 @@
         <v>79</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="3">
@@ -3800,21 +3798,21 @@
         <v>79</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3">
@@ -3825,21 +3823,21 @@
         <v>79</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3">
@@ -3850,21 +3848,21 @@
         <v>79</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3">
@@ -3875,21 +3873,21 @@
         <v>79</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3">
@@ -3900,21 +3898,21 @@
         <v>79</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3">
@@ -3925,18 +3923,18 @@
         <v>79</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>42</v>
@@ -3947,21 +3945,21 @@
       </c>
       <c r="G97" s="3"/>
       <c r="H97" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>42</v>
@@ -3972,21 +3970,21 @@
       </c>
       <c r="G98" s="3"/>
       <c r="H98" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>42</v>
@@ -3997,21 +3995,21 @@
       </c>
       <c r="G99" s="3"/>
       <c r="H99" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C100" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>42</v>
@@ -4026,13 +4024,13 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C101" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>42</v>
@@ -4047,13 +4045,13 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C102" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>42</v>
@@ -4068,13 +4066,13 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C103" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>42</v>
@@ -4089,13 +4087,13 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C104" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>42</v>
@@ -4110,13 +4108,13 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C105" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>42</v>
@@ -4131,13 +4129,13 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C106" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>42</v>
@@ -4152,13 +4150,13 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C107" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>42</v>
@@ -4173,13 +4171,13 @@
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="3" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C108" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>42</v>
@@ -4194,13 +4192,13 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="3" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C109" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>42</v>
@@ -4215,13 +4213,13 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C110" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>42</v>
@@ -4236,13 +4234,13 @@
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C111" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>42</v>
@@ -4257,13 +4255,13 @@
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="3" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C112" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>42</v>
@@ -4276,243 +4274,243 @@
       </c>
       <c r="J112" s="3"/>
     </row>
-    <row r="113" spans="1:10" s="18" customFormat="1">
-      <c r="A113" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="B113" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C113" s="18" t="s">
+    <row r="113" spans="1:10">
+      <c r="A113" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="D113" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E113" s="17"/>
-      <c r="F113" s="17"/>
-      <c r="G113" s="17"/>
-      <c r="H113" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J113" s="17"/>
-    </row>
-    <row r="114" spans="1:10" s="18" customFormat="1">
-      <c r="A114" s="17" t="s">
+      <c r="B113" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C113" t="s">
         <v>306</v>
       </c>
-      <c r="B114" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C114" s="18" t="s">
+      <c r="D113" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J113" s="3"/>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D114" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-      <c r="G114" s="17"/>
-      <c r="H114" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J114" s="17" t="s">
+      <c r="B114" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C114" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" s="18" customFormat="1">
-      <c r="A115" s="17" t="s">
+      <c r="D114" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
+      <c r="H114" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J114" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="B115" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C115" s="18" t="s">
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="D115" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E115" s="17"/>
-      <c r="F115" s="17"/>
-      <c r="G115" s="17"/>
-      <c r="H115" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J115" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" s="18" customFormat="1">
-      <c r="A116" s="17" t="s">
+      <c r="B115" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C115" t="s">
         <v>311</v>
       </c>
-      <c r="B116" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C116" s="18" t="s">
+      <c r="D115" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="D116" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E116" s="17"/>
-      <c r="F116" s="17"/>
-      <c r="G116" s="17"/>
-      <c r="H116" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J116" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" s="18" customFormat="1">
-      <c r="A117" s="17" t="s">
+      <c r="B116" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C116" t="s">
         <v>313</v>
       </c>
-      <c r="B117" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C117" s="18" t="s">
+      <c r="D116" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="D117" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E117" s="17"/>
-      <c r="F117" s="17"/>
-      <c r="G117" s="17"/>
-      <c r="H117" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J117" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" s="18" customFormat="1">
-      <c r="A118" s="17" t="s">
+      <c r="B117" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C117" t="s">
         <v>315</v>
       </c>
-      <c r="B118" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C118" s="18" t="s">
+      <c r="D117" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D118" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E118" s="17"/>
-      <c r="F118" s="17"/>
-      <c r="G118" s="17"/>
-      <c r="H118" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J118" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" s="18" customFormat="1">
-      <c r="A119" s="17" t="s">
+      <c r="B118" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C118" t="s">
         <v>317</v>
       </c>
-      <c r="B119" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C119" s="18" t="s">
+      <c r="D118" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="D119" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E119" s="17"/>
-      <c r="F119" s="17"/>
-      <c r="G119" s="17"/>
-      <c r="H119" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J119" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" s="18" customFormat="1">
-      <c r="A120" s="17" t="s">
+      <c r="B119" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C119" t="s">
         <v>319</v>
       </c>
-      <c r="B120" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C120" s="18" t="s">
+      <c r="D119" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
+      <c r="H119" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D120" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E120" s="17"/>
-      <c r="F120" s="17"/>
-      <c r="G120" s="17"/>
-      <c r="H120" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J120" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" s="18" customFormat="1">
-      <c r="A121" s="17" t="s">
+      <c r="B120" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C120" t="s">
         <v>321</v>
       </c>
-      <c r="B121" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C121" s="18" t="s">
+      <c r="D120" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
+      <c r="H120" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J120" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="D121" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E121" s="17"/>
-      <c r="F121" s="17"/>
-      <c r="G121" s="17"/>
-      <c r="H121" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J121" s="17" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" s="18" customFormat="1">
-      <c r="A122" s="17" t="s">
+      <c r="B121" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C121" t="s">
         <v>323</v>
       </c>
-      <c r="B122" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C122" s="18" t="s">
+      <c r="D121" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J121" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="D122" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E122" s="17"/>
-      <c r="F122" s="17"/>
-      <c r="G122" s="17"/>
-      <c r="H122" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J122" s="17" t="s">
-        <v>308</v>
+      <c r="B122" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C122" t="s">
+        <v>325</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J122" s="3" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="123" spans="1:10" s="10" customFormat="1">
       <c r="A123" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>42</v>
@@ -4521,46 +4519,55 @@
       <c r="F123" s="9"/>
       <c r="G123" s="9"/>
       <c r="H123" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J123" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B124" t="s">
-        <v>329</v>
+        <v>330</v>
+      </c>
+      <c r="D124" t="s">
+        <v>42</v>
       </c>
       <c r="F124">
         <v>927</v>
       </c>
       <c r="J124" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B125" t="s">
-        <v>329</v>
+        <v>330</v>
+      </c>
+      <c r="D125" t="s">
+        <v>42</v>
       </c>
       <c r="F125">
         <v>927</v>
       </c>
       <c r="J125" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B126" t="s">
-        <v>329</v>
+        <v>330</v>
+      </c>
+      <c r="D126" t="s">
+        <v>42</v>
       </c>
       <c r="F126">
         <v>927</v>
@@ -4568,10 +4575,13 @@
     </row>
     <row r="127" spans="1:10">
       <c r="A127" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B127" t="s">
-        <v>329</v>
+        <v>330</v>
+      </c>
+      <c r="D127" t="s">
+        <v>42</v>
       </c>
       <c r="F127">
         <v>927</v>
@@ -4579,10 +4589,13 @@
     </row>
     <row r="128" spans="1:10">
       <c r="A128" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B128" t="s">
-        <v>329</v>
+        <v>330</v>
+      </c>
+      <c r="D128" t="s">
+        <v>42</v>
       </c>
       <c r="F128">
         <v>927</v>
@@ -4590,26 +4603,19 @@
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B129" t="s">
-        <v>329</v>
+        <v>330</v>
+      </c>
+      <c r="D129" t="s">
+        <v>42</v>
       </c>
       <c r="F129">
         <v>927</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
-      <c r="A130" t="s">
-        <v>337</v>
-      </c>
-      <c r="B130" t="s">
-        <v>329</v>
-      </c>
-      <c r="F130">
-        <v>927</v>
-      </c>
-    </row>
+    <row r="130" spans="1:6"/>
     <row r="131" spans="1:6"/>
     <row r="132" spans="1:6"/>
     <row r="133" spans="1:6"/>

</xml_diff>